<commit_message>
BWP Test Cases and Keywords added
</commit_message>
<xml_diff>
--- a/KatalonData/BWPBootstrapData/BWPCCData.xlsx
+++ b/KatalonData/BWPBootstrapData/BWPCCData.xlsx
@@ -1,25 +1,170 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\BWPBootstrapData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{C9BF4F9A-767C-4F42-9207-1210B83744AC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="7" firstSheet="4" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PayNowCCNoCF" r:id="rId1" sheetId="1"/>
+    <sheet name="PayNowCCNoCFReqFields" r:id="rId2" sheetId="2"/>
+    <sheet name="PayNowCCSCF" r:id="rId3" sheetId="3"/>
+    <sheet name="PayNowCCDCF" r:id="rId4" sheetId="4"/>
+    <sheet name="PayNowCCNoCFOnly" r:id="rId5" sheetId="5"/>
+    <sheet name="NoModifyAmountCC" r:id="rId6" sheetId="6"/>
+    <sheet name="MaxAmountErrorCC" r:id="rId7" sheetId="7"/>
+    <sheet name="MinAmountErrorCC" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="42">
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>EmulatorData</t>
+  </si>
+  <si>
+    <t>AppID</t>
+  </si>
+  <si>
+    <t>MessageVersion</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>UDFID</t>
+  </si>
+  <si>
+    <t>NameID</t>
+  </si>
+  <si>
+    <t>CardID</t>
+  </si>
+  <si>
+    <t>CalDate</t>
+  </si>
+  <si>
+    <t>AddressID</t>
+  </si>
+  <si>
+    <t>EmailPhoneID</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 19:36:46 IST 2025</t>
+  </si>
+  <si>
+    <t>951</t>
+  </si>
+  <si>
+    <t>952</t>
+  </si>
+  <si>
+    <t>10.50</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tue Sep 30 22:32:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 01 19:05:22 IST 2025</t>
+  </si>
+  <si>
+    <t>954</t>
+  </si>
+  <si>
+    <t>Fri Oct 03 20:19:23 IST 2025</t>
+  </si>
+  <si>
+    <t>956</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Tue Oct 07 21:24:00 IST 2025</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Wed Oct 08 20:32:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 08 20:38:58 IST 2025</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Oct 09 19:24:13 IST 2025</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,18 +190,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -73,10 +237,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -111,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -240,21 +404,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -271,7 +435,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -323,20 +487,789 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2AA229-8633-483E-A009-0064BA327142}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BFFB65-1565-4A34-B0E7-464EF87C75A7}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125BE3DD-7AC0-404A-8C39-EB8ECFFFBDDD}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE94437-153A-41B2-A46E-2F45E61989DF}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093A05D5-CD46-4FC8-83C2-DE55EC3B00E1}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6F3014-83EE-40CF-BEA6-9E7A762354AA}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434CAF96-FDCD-425D-B74E-26C08061546A}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>